<commit_message>
Renaming file convention and removing while loop step up
</commit_message>
<xml_diff>
--- a/ListofPersonalities.xlsx
+++ b/ListofPersonalities.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh16.Yadav\Desktop\github\Personalities_Python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890BF47B-E2F0-4915-B353-A67E50494850}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{2121B60F-749E-41FA-9635-D96375D737BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15350" windowHeight="4470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProminentPersonalities" sheetId="1" r:id="rId1"/>
     <sheet name="Objects" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Yogi Adityanath</t>
   </si>
@@ -319,17 +313,38 @@
     <t>Categories</t>
   </si>
   <si>
-    <t xml:space="preserve">People Wearing Nehru Jacket </t>
-  </si>
-  <si>
     <t>Football Images</t>
+  </si>
+  <si>
+    <t>Smiling Face</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nehru Jacket </t>
+  </si>
+  <si>
+    <t>Glasses</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Birds</t>
+  </si>
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Car</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,7 +464,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -501,7 +516,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -695,501 +710,501 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA8C736-432D-4EC2-9A7C-EE7F8D1C4B6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -1201,26 +1216,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EE2373-C393-475C-A9B1-4DABD6D164DB}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>